<commit_message>
Fix getHyperlinkFunctionCellAddress in DefaultHyperlinkCellClickHandler (#43)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/spreadsheet_hyperlinks.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/spreadsheet_hyperlinks.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -47,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -76,12 +76,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -104,15 +98,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -465,7 +458,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -480,11 +473,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="str">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="str">
         <f>HYPERLINK(G1,F1)</f>
         <v>google</v>
       </c>
@@ -497,16 +490,16 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="5" t="str">
+      <c r="I2" s="3" t="str">
         <f>HYPERLINK(G2,F2)</f>
         <v>gmail</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -517,7 +510,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5">
@@ -525,30 +518,40 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="str">
+      <c r="A6" s="2" t="str">
         <f>HYPERLINK("[spreadsheet_hyperlinks.xlsx]Sheet1!B6", "explicit link to next cell")</f>
         <v>explicit link to next cell</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="C7" s="1" t="str">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="str">
+        <f>HYPERLINK( "http://www.google.com" )</f>
+        <v>http://www.google.com</v>
+      </c>
+      <c r="C7" s="4" t="str">
         <f>HYPERLINK("http://www.google.com",  "merged cell link")</f>
         <v>merged cell link</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="str">
+        <f>HYPERLINK(( "http://www.google.com" ))</f>
+        <v>http://www.google.com</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="str">
+        <f>HYPERLINK(("http://www.google.com")   )</f>
+        <v>http://www.google.com</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E11">

</xml_diff>